<commit_message>
Forgot to update PoS baselines
</commit_message>
<xml_diff>
--- a/results/acl-pretrain/baselines_pos.xlsx
+++ b/results/acl-pretrain/baselines_pos.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aturt\Documents\typology_of_crosslingual\results\acl-pretrain\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -78,8 +73,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,19 +137,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -196,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,10 +215,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -263,7 +249,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -439,16 +424,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,132 +439,132 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.19619522556217389</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.2118068965517241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.20301448299090599</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.1805458229957766</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.25214921707092408</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.2521492170709241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.18277381031836079</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.1827738103183608</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.21049258377586519</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.2104925837758652</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.25262666355358387</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.2757242757242757</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.32103722291928072</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.3210372229192807</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.27112265925992302</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.271122659259923</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.23581863979848869</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.216893039049236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.26688997029640399</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.2738805263656158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.24850250266677609</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.2485025026667761</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.48733719247467439</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.2939434534301629</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.24259557419403149</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.2832591683289857</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.37007599930382318</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.2672127950068266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.26880632258686332</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.2971181376820615</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.20261610622976811</v>
+        <v>0.2026161062297681</v>
       </c>
     </row>
   </sheetData>

</xml_diff>